<commit_message>
Merge cells in report
</commit_message>
<xml_diff>
--- a/public/hello world.xlsx
+++ b/public/hello world.xlsx
@@ -399,6 +399,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -467,6 +470,19 @@
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A46:F46"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>